<commit_message>
Ran Test on Web App
</commit_message>
<xml_diff>
--- a/Web Application User Acceptance Testing/CMPG323 EcoPower Logistics Data.xlsx
+++ b/Web Application User Acceptance Testing/CMPG323 EcoPower Logistics Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\armin\Documents\GitHub\CMPG323-Project-4-34739572\Web Application User Acceptance Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30B242D-1D8C-43AF-BC79-9B7EA7677AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4B6ABB-B5A3-4BB2-8B8C-5E7C60571DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2265" yWindow="2535" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="114">
   <si>
     <t>CustomerId</t>
   </si>
@@ -378,6 +378,9 @@
   </si>
   <si>
     <t>Test Result</t>
+  </si>
+  <si>
+    <t>Success</t>
   </si>
 </sst>
 </file>
@@ -733,7 +736,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F14"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,6 +782,9 @@
       <c r="E2">
         <v>5723177115</v>
       </c>
+      <c r="F2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -796,6 +802,9 @@
       <c r="E3">
         <v>9041993848</v>
       </c>
+      <c r="F3" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -813,6 +822,9 @@
       <c r="E4">
         <v>3738283528</v>
       </c>
+      <c r="F4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -830,6 +842,9 @@
       <c r="E5">
         <v>6447102299</v>
       </c>
+      <c r="F5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -847,6 +862,9 @@
       <c r="E6">
         <v>1878764468</v>
       </c>
+      <c r="F6" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -864,6 +882,9 @@
       <c r="E7">
         <v>9666552669</v>
       </c>
+      <c r="F7" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -881,6 +902,9 @@
       <c r="E8">
         <v>2384982848</v>
       </c>
+      <c r="F8" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -898,6 +922,9 @@
       <c r="E9">
         <v>8945409882</v>
       </c>
+      <c r="F9" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -915,6 +942,9 @@
       <c r="E10">
         <v>1320602595</v>
       </c>
+      <c r="F10" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -932,6 +962,9 @@
       <c r="E11">
         <v>7968612324</v>
       </c>
+      <c r="F11" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -949,6 +982,9 @@
       <c r="E12">
         <v>1578247192</v>
       </c>
+      <c r="F12" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -966,6 +1002,9 @@
       <c r="E13">
         <v>7425817353</v>
       </c>
+      <c r="F13" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -982,6 +1021,9 @@
       </c>
       <c r="E14">
         <v>5815761997</v>
+      </c>
+      <c r="F14" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -993,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,6 +1084,9 @@
       <c r="E2">
         <v>0</v>
       </c>
+      <c r="F2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1059,6 +1104,9 @@
       <c r="E3">
         <v>0</v>
       </c>
+      <c r="F3" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1076,6 +1124,9 @@
       <c r="E4">
         <v>0</v>
       </c>
+      <c r="F4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1093,6 +1144,9 @@
       <c r="E5">
         <v>0</v>
       </c>
+      <c r="F5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1110,6 +1164,9 @@
       <c r="E6">
         <v>0.7</v>
       </c>
+      <c r="F6" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1127,6 +1184,9 @@
       <c r="E7">
         <v>0.2</v>
       </c>
+      <c r="F7" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1144,6 +1204,9 @@
       <c r="E8">
         <v>0.2</v>
       </c>
+      <c r="F8" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1161,6 +1224,9 @@
       <c r="E9">
         <v>0.2</v>
       </c>
+      <c r="F9" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1178,6 +1244,9 @@
       <c r="E10">
         <v>0.2</v>
       </c>
+      <c r="F10" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1195,6 +1264,9 @@
       <c r="E11">
         <v>0.2</v>
       </c>
+      <c r="F11" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1212,6 +1284,9 @@
       <c r="E12">
         <v>0.2</v>
       </c>
+      <c r="F12" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1229,6 +1304,9 @@
       <c r="E13">
         <v>0.2</v>
       </c>
+      <c r="F13" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1246,6 +1324,9 @@
       <c r="E14">
         <v>0</v>
       </c>
+      <c r="F14" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1263,6 +1344,9 @@
       <c r="E15">
         <v>0</v>
       </c>
+      <c r="F15" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1280,8 +1364,11 @@
       <c r="E16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6091</v>
       </c>
@@ -1297,8 +1384,11 @@
       <c r="E17">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6092</v>
       </c>
@@ -1314,8 +1404,11 @@
       <c r="E18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6093</v>
       </c>
@@ -1331,8 +1424,11 @@
       <c r="E19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6094</v>
       </c>
@@ -1348,8 +1444,11 @@
       <c r="E20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6095</v>
       </c>
@@ -1365,8 +1464,11 @@
       <c r="E21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6096</v>
       </c>
@@ -1382,8 +1484,11 @@
       <c r="E22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6097</v>
       </c>
@@ -1399,8 +1504,11 @@
       <c r="E23">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6098</v>
       </c>
@@ -1416,8 +1524,11 @@
       <c r="E24">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6099</v>
       </c>
@@ -1433,8 +1544,11 @@
       <c r="E25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6100</v>
       </c>
@@ -1450,8 +1564,11 @@
       <c r="E26">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>6101</v>
       </c>
@@ -1467,8 +1584,11 @@
       <c r="E27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6102</v>
       </c>
@@ -1484,8 +1604,11 @@
       <c r="E28">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6103</v>
       </c>
@@ -1501,8 +1624,11 @@
       <c r="E29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6104</v>
       </c>
@@ -1518,8 +1644,11 @@
       <c r="E30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>6288</v>
       </c>
@@ -1535,8 +1664,11 @@
       <c r="E31">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6289</v>
       </c>
@@ -1552,8 +1684,11 @@
       <c r="E32">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7320</v>
       </c>
@@ -1569,8 +1704,11 @@
       <c r="E33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7321</v>
       </c>
@@ -1586,8 +1724,11 @@
       <c r="E34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>7404</v>
       </c>
@@ -1603,8 +1744,11 @@
       <c r="E35">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>7405</v>
       </c>
@@ -1620,8 +1764,11 @@
       <c r="E36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>7406</v>
       </c>
@@ -1637,8 +1784,11 @@
       <c r="E37">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>7407</v>
       </c>
@@ -1654,8 +1804,11 @@
       <c r="E38">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>9132</v>
       </c>
@@ -1671,8 +1824,11 @@
       <c r="E39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>9133</v>
       </c>
@@ -1688,8 +1844,11 @@
       <c r="E40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>9737</v>
       </c>
@@ -1704,6 +1863,9 @@
       </c>
       <c r="E41">
         <v>0</v>
+      </c>
+      <c r="F41" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1758,6 +1920,9 @@
       <c r="D2" t="s">
         <v>43</v>
       </c>
+      <c r="E2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1772,6 +1937,9 @@
       <c r="D3" t="s">
         <v>44</v>
       </c>
+      <c r="E3" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1786,6 +1954,9 @@
       <c r="D4" t="s">
         <v>45</v>
       </c>
+      <c r="E4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1800,6 +1971,9 @@
       <c r="D5" t="s">
         <v>46</v>
       </c>
+      <c r="E5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1814,6 +1988,9 @@
       <c r="D6" t="s">
         <v>47</v>
       </c>
+      <c r="E6" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1828,6 +2005,9 @@
       <c r="D7" t="s">
         <v>48</v>
       </c>
+      <c r="E7" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1842,6 +2022,9 @@
       <c r="D8" t="s">
         <v>49</v>
       </c>
+      <c r="E8" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1856,6 +2039,9 @@
       <c r="D9" t="s">
         <v>50</v>
       </c>
+      <c r="E9" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1870,6 +2056,9 @@
       <c r="D10" t="s">
         <v>51</v>
       </c>
+      <c r="E10" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1884,6 +2073,9 @@
       <c r="D11" t="s">
         <v>52</v>
       </c>
+      <c r="E11" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1898,6 +2090,9 @@
       <c r="D12" t="s">
         <v>53</v>
       </c>
+      <c r="E12" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1912,6 +2107,9 @@
       <c r="D13" t="s">
         <v>54</v>
       </c>
+      <c r="E13" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1926,6 +2124,9 @@
       <c r="D14" t="s">
         <v>55</v>
       </c>
+      <c r="E14" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1939,6 +2140,9 @@
       </c>
       <c r="D15" t="s">
         <v>56</v>
+      </c>
+      <c r="E15" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1950,8 +2154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F2:F7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1993,6 +2197,9 @@
       <c r="D2">
         <v>950</v>
       </c>
+      <c r="E2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -2007,6 +2214,9 @@
       <c r="D3">
         <v>61</v>
       </c>
+      <c r="E3" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -2021,6 +2231,9 @@
       <c r="D4">
         <v>281</v>
       </c>
+      <c r="E4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -2035,6 +2248,9 @@
       <c r="D5">
         <v>502</v>
       </c>
+      <c r="E5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -2049,6 +2265,9 @@
       <c r="D6">
         <v>621</v>
       </c>
+      <c r="E6" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -2063,6 +2282,9 @@
       <c r="D7">
         <v>765</v>
       </c>
+      <c r="E7" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -2077,6 +2299,9 @@
       <c r="D8">
         <v>709</v>
       </c>
+      <c r="E8" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -2091,6 +2316,9 @@
       <c r="D9">
         <v>485</v>
       </c>
+      <c r="E9" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -2105,6 +2333,9 @@
       <c r="D10">
         <v>158</v>
       </c>
+      <c r="E10" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -2119,6 +2350,9 @@
       <c r="D11">
         <v>485</v>
       </c>
+      <c r="E11" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -2133,6 +2367,9 @@
       <c r="D12">
         <v>322</v>
       </c>
+      <c r="E12" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -2147,6 +2384,9 @@
       <c r="D13">
         <v>51</v>
       </c>
+      <c r="E13" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -2161,6 +2401,9 @@
       <c r="D14">
         <v>152</v>
       </c>
+      <c r="E14" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -2175,6 +2418,9 @@
       <c r="D15">
         <v>634</v>
       </c>
+      <c r="E15" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -2189,8 +2435,11 @@
       <c r="D16">
         <v>299</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10001606</v>
       </c>
@@ -2203,8 +2452,11 @@
       <c r="D17">
         <v>466</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10001622</v>
       </c>
@@ -2217,8 +2469,11 @@
       <c r="D18">
         <v>971</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10001772</v>
       </c>
@@ -2231,8 +2486,11 @@
       <c r="D19">
         <v>434</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10001979</v>
       </c>
@@ -2245,8 +2503,11 @@
       <c r="D20">
         <v>228</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10001998</v>
       </c>
@@ -2259,8 +2520,11 @@
       <c r="D21">
         <v>142</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10002012</v>
       </c>
@@ -2273,8 +2537,11 @@
       <c r="D22">
         <v>789</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10002310</v>
       </c>
@@ -2287,8 +2554,11 @@
       <c r="D23">
         <v>924</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10002475</v>
       </c>
@@ -2301,8 +2571,11 @@
       <c r="D24">
         <v>206</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>10002563</v>
       </c>
@@ -2315,8 +2588,11 @@
       <c r="D25">
         <v>832</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>10002647</v>
       </c>
@@ -2329,8 +2605,11 @@
       <c r="D26">
         <v>712</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>10002713</v>
       </c>
@@ -2343,8 +2622,11 @@
       <c r="D27">
         <v>781</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>10002885</v>
       </c>
@@ -2357,8 +2639,11 @@
       <c r="D28">
         <v>977</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10002968</v>
       </c>
@@ -2371,8 +2656,11 @@
       <c r="D29">
         <v>95</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>10003012</v>
       </c>
@@ -2385,8 +2673,11 @@
       <c r="D30">
         <v>315</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>10003061</v>
       </c>
@@ -2399,8 +2690,11 @@
       <c r="D31">
         <v>433</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>10003072</v>
       </c>
@@ -2413,8 +2707,11 @@
       <c r="D32">
         <v>495</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>10003623</v>
       </c>
@@ -2427,8 +2724,11 @@
       <c r="D33">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>10003715</v>
       </c>
@@ -2441,8 +2741,11 @@
       <c r="D34">
         <v>263</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>10003833</v>
       </c>
@@ -2455,8 +2758,11 @@
       <c r="D35">
         <v>810</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>10003846</v>
       </c>
@@ -2469,8 +2775,11 @@
       <c r="D36">
         <v>637</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>10004015</v>
       </c>
@@ -2483,8 +2792,11 @@
       <c r="D37">
         <v>804</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>10004086</v>
       </c>
@@ -2497,8 +2809,11 @@
       <c r="D38">
         <v>933</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>10004495</v>
       </c>
@@ -2511,8 +2826,11 @@
       <c r="D39">
         <v>595</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>10004667</v>
       </c>
@@ -2524,6 +2842,9 @@
       </c>
       <c r="D40">
         <v>557</v>
+      </c>
+      <c r="E40" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hotfix, Publish and Test
</commit_message>
<xml_diff>
--- a/Web Application User Acceptance Testing/CMPG323 EcoPower Logistics Data.xlsx
+++ b/Web Application User Acceptance Testing/CMPG323 EcoPower Logistics Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\armin\Documents\GitHub\CMPG323-Project-4-34739572\Web Application User Acceptance Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4B6ABB-B5A3-4BB2-8B8C-5E7C60571DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F3083D-2F55-439F-BE49-2AB3F6D36B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -736,7 +736,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="F20" sqref="F2:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1878,7 +1878,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E17" sqref="E2:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2155,7 +2155,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>